<commit_message>
more data from cellprofiler
</commit_message>
<xml_diff>
--- a/rad_pipeline/week_one_cells_layout.xlsx
+++ b/rad_pipeline/week_one_cells_layout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t>Location</t>
   </si>
@@ -82,6 +82,18 @@
     <t>r08c11</t>
   </si>
   <si>
+    <t>r07c09</t>
+  </si>
+  <si>
+    <t>r07c11</t>
+  </si>
+  <si>
+    <t>r08c10</t>
+  </si>
+  <si>
+    <t>r08c12</t>
+  </si>
+  <si>
     <t>r01c01</t>
   </si>
   <si>
@@ -122,9 +134,6 @@
   </si>
   <si>
     <t>r03c03</t>
-  </si>
-  <si>
-    <t>Compound_0</t>
   </si>
   <si>
     <t>Compound_4</t>
@@ -1823,7 +1832,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>0.01</v>
@@ -1831,7 +1840,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>0.01</v>
@@ -1839,7 +1848,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>0.01</v>
@@ -1847,7 +1856,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>0.01</v>
@@ -2860,10 +2869,10 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -2871,15 +2880,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -2887,31 +2896,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -2919,15 +2928,15 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -2935,79 +2944,79 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -3015,15 +3024,15 @@
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -3031,15 +3040,15 @@
         <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -3047,7 +3056,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -4062,154 +4071,154 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -4217,15 +4226,15 @@
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -4233,23 +4242,23 @@
         <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>

</xml_diff>